<commit_message>
Auto commit from script
</commit_message>
<xml_diff>
--- a/test-data/testData.xlsx
+++ b/test-data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HybridFramework\HybridFramework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9538E43-303D-4A19-A482-498C814AEDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3832BA19-E0AA-4EDD-BCA8-9029496CEA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{D0ED6061-E5DD-403A-88F5-76EEA8FB5438}"/>
   </bookViews>
@@ -36,12 +36,75 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>usertype</t>
+  </si>
+  <si>
+    <t>userrole</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t> rahulshettyacademy</t>
+  </si>
+  <si>
+    <t>learning</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>rahul@shetty</t>
+  </si>
+  <si>
+    <t>lear#@ing</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,13 +127,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,14 +457,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D99DF5A-14D1-47AF-B0E7-F58C73B15F07}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{E997A326-C325-4D4D-984E-29839D0FF56C}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{3633C354-1BDB-407B-8188-E07EB52DD6B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>